<commit_message>
Variables de exportaciones e importaciones añadidas
</commit_message>
<xml_diff>
--- a/data/precios-agroquimicos-fertilizantes.xlsx
+++ b/data/precios-agroquimicos-fertilizantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a98dfaf1ce87dfc/DataScience/Proyectos/time-series-fertilizer-price-predictor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{F10DE583-1609-43F1-A029-7C2CD5B85C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14DEC7A1-7A84-4D47-9999-02B7A5158FE5}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{F10DE583-1609-43F1-A029-7C2CD5B85C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C54FB3E4-D2CA-4FDD-B30D-4F56A818B3F0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="642" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="642" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ÍNDICE" sheetId="15" r:id="rId1"/>
@@ -1911,9 +1911,6 @@
     <t>El modelo de regularización y control de precios de los insumos agropecuarios es un mecanismo que logrará identificar los limites maximos y minimos de los precios de comercialización de los insumos en el territorio nacional. Con la finalidad de deterinar posibles sobreprecios y especulaciónes de las principales empresas comercializadores en el país.</t>
   </si>
   <si>
-    <t>úrea</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -1921,6 +1918,9 @@
   </si>
   <si>
     <t>muriato_de_potasio</t>
+  </si>
+  <si>
+    <t>urea</t>
   </si>
 </sst>
 </file>
@@ -2903,11 +2903,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3623,15 +3623,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -3654,15 +3654,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -3685,17 +3685,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -3749,16 +3749,16 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="135" t="s">
@@ -3770,32 +3770,32 @@
       <c r="I8" s="135"/>
       <c r="J8" s="135"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="15" t="s">
         <v>72</v>
       </c>
@@ -5533,11 +5533,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:G5"/>
     <mergeCell ref="A6:M6"/>
     <mergeCell ref="L8:Q8"/>
     <mergeCell ref="R8:AA8"/>
@@ -5546,6 +5541,11 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:J8"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="ÍNDICE!A1" display="ÍNDICE" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
@@ -5596,15 +5596,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -5627,15 +5627,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -5658,17 +5658,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -5722,16 +5722,16 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="135" t="s">
@@ -5743,32 +5743,32 @@
       <c r="I8" s="135"/>
       <c r="J8" s="135"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="15" t="s">
         <v>72</v>
       </c>
@@ -7545,15 +7545,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -7576,15 +7576,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -7607,13 +7607,13 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
       <c r="F5" s="5" t="s">
         <v>109</v>
       </c>
@@ -7654,16 +7654,16 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="135" t="s">
@@ -7675,32 +7675,32 @@
       <c r="I8" s="135"/>
       <c r="J8" s="135"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="36.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="15" t="s">
         <v>72</v>
       </c>
@@ -9428,6 +9428,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A6:M6"/>
     <mergeCell ref="R8:AA8"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
@@ -9435,11 +9440,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:J8"/>
     <mergeCell ref="L8:Q8"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A6:M6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="ÍNDICE!A1" display="ÍNDICE" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
@@ -9599,16 +9599,16 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="135" t="s">
@@ -9620,32 +9620,32 @@
       <c r="I8" s="135"/>
       <c r="J8" s="135"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="36.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="15" t="s">
         <v>72</v>
       </c>
@@ -11501,13 +11501,13 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:28" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="134" t="s">
@@ -11522,34 +11522,34 @@
       <c r="I8" s="135"/>
       <c r="J8" s="135"/>
       <c r="K8" s="96"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
       <c r="Q8" s="134"/>
-      <c r="R8" s="131" t="s">
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
       <c r="AA8" s="134"/>
       <c r="AB8" s="23" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="36.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="134"/>
       <c r="E9" s="15" t="s">
         <v>72</v>
@@ -13316,7 +13316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:EF81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
       <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
@@ -19689,7 +19689,7 @@
     <row r="25" spans="1:136" s="7" customFormat="1">
       <c r="A25" s="128"/>
       <c r="B25" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="43" t="s">
         <v>24</v>
@@ -20716,8 +20716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4CFAB7-A2C5-4416-961C-320A58A19CEC}">
   <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -20728,16 +20728,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="115" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="C1" s="116" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="D1" s="116" t="s">
         <v>139</v>
-      </c>
-      <c r="D1" s="116" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -22634,15 +22634,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -22665,15 +22665,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -22696,17 +22696,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -22760,53 +22760,53 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="134"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="17" t="s">
         <v>72</v>
       </c>
@@ -24372,6 +24372,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R8:AA8"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A3:G3"/>
@@ -24380,11 +24385,6 @@
     <mergeCell ref="E8:K8"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:M6"/>
-    <mergeCell ref="R8:AA8"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="ÍNDICE!A1" display="ÍNDICE" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -24437,15 +24437,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -24468,15 +24468,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -24499,17 +24499,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -24563,53 +24563,53 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="134"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="17" t="s">
         <v>72</v>
       </c>
@@ -26269,11 +26269,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="D1:I1"/>
     <mergeCell ref="A6:M6"/>
     <mergeCell ref="R8:AA8"/>
     <mergeCell ref="A8:A9"/>
@@ -26282,6 +26277,11 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:K8"/>
     <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="D1:I1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="ÍNDICE!A1" display="ÍNDICE" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -26334,15 +26334,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -26365,15 +26365,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -26396,17 +26396,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -26460,53 +26460,53 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="134"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="17" t="s">
         <v>72</v>
       </c>
@@ -28299,15 +28299,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -28330,15 +28330,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -28361,17 +28361,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -28425,53 +28425,53 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="134"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="17" t="s">
         <v>72</v>
       </c>
@@ -30253,15 +30253,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -30284,15 +30284,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -30315,17 +30315,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -30379,53 +30379,53 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
       <c r="K8" s="134"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="17" t="s">
         <v>72</v>
       </c>
@@ -32174,15 +32174,15 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -32205,15 +32205,15 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -32236,17 +32236,17 @@
       <c r="AA4" s="5"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -32300,16 +32300,16 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C8" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="131" t="s">
+      <c r="D8" s="132" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="135" t="s">
@@ -32321,32 +32321,32 @@
       <c r="I8" s="135"/>
       <c r="J8" s="135"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131" t="s">
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="132"/>
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
     </row>
     <row r="9" spans="1:27" ht="24.6" thickBot="1">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="15" t="s">
         <v>72</v>
       </c>

</xml_diff>